<commit_message>
change -1 to 0 in gap column for individual propeller
</commit_message>
<xml_diff>
--- a/validate_data/corotatingBlades/corotating_data.xlsx
+++ b/validate_data/corotatingBlades/corotating_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28785" windowHeight="13395"/>
+    <workbookView windowWidth="28800" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1279,7 +1279,7 @@
   <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1395,7 +1395,7 @@
         <v>31</v>
       </c>
       <c r="B2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1418,7 +1418,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1441,7 +1441,7 @@
         <v>31</v>
       </c>
       <c r="B4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>

</xml_diff>